<commit_message>
Adjust New Dummy Database
</commit_message>
<xml_diff>
--- a/files/templates/Template - Dummy Database.xlsx
+++ b/files/templates/Template - Dummy Database.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data Analytical\PROJECT\REQUEST\20250626_Automate DB Update IOH\Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data Analytical\PROJECT\REQUEST\20250626_Automate DB Update IOH\files\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8733700-353D-44C8-BA13-B724E8289C05}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B14AF47-A557-4A07-8795-13B1FB952208}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" xr2:uid="{015C3B1C-0D0B-4B59-9E69-D8A4A7569914}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" activeTab="1" xr2:uid="{015C3B1C-0D0B-4B59-9E69-D8A4A7569914}"/>
   </bookViews>
   <sheets>
     <sheet name="Site List" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="179">
   <si>
     <t>Ring ID</t>
   </si>
@@ -1063,8 +1063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71FA8DEF-346F-4FF8-B679-7B2C9BBEBF84}">
   <dimension ref="A1:S19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2039,8 +2039,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{758C3781-8904-47B4-8E4D-887B382677C7}">
   <dimension ref="A1:V19"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3259,7 +3259,7 @@
         <v>129</v>
       </c>
       <c r="L18" s="17" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="M18" s="15" t="s">
         <v>132</v>
@@ -3324,13 +3324,13 @@
         <v>163</v>
       </c>
       <c r="K19" s="17" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="L19" s="17" t="s">
         <v>126</v>
       </c>
       <c r="M19" s="15" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N19" s="15">
         <v>11773</v>
@@ -3344,11 +3344,21 @@
       <c r="Q19" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="R19" s="15"/>
-      <c r="S19" s="15"/>
-      <c r="T19" s="15"/>
-      <c r="U19" s="15"/>
-      <c r="V19" s="15"/>
+      <c r="R19" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="S19" s="15">
+        <v>2100</v>
+      </c>
+      <c r="T19" s="15">
+        <v>1000</v>
+      </c>
+      <c r="U19" s="15">
+        <v>3100</v>
+      </c>
+      <c r="V19" s="15" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>